<commit_message>
Old data + Mahasangram
</commit_message>
<xml_diff>
--- a/Registration list till 4 nov.xlsx
+++ b/Registration list till 4 nov.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DYPU Sports Committee\dypusportscommittee\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{7392DB9F-D781-4E1A-8903-1E38F539D952}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E201EED7-3A45-4E51-B8AA-C9CBAA17512B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" activeTab="3" xr2:uid="{B784C5FB-534E-4FF5-8A1E-3B229C06DE26}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{B784C5FB-534E-4FF5-8A1E-3B229C06DE26}"/>
   </bookViews>
   <sheets>
     <sheet name="Cricket" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="214" uniqueCount="87">
   <si>
     <t>Name</t>
   </si>
@@ -120,9 +120,6 @@
     <t>Aryan Keni</t>
   </si>
   <si>
-    <t xml:space="preserve">Priyanshi Jakharia </t>
-  </si>
-  <si>
     <t>Manav Bothe</t>
   </si>
   <si>
@@ -265,13 +262,49 @@
   </si>
   <si>
     <t>meet samwadkar</t>
+  </si>
+  <si>
+    <t>500 UPI 50 Cash</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Priyanshi Jakhaaria </t>
+  </si>
+  <si>
+    <t>Nidhi Thakkar</t>
+  </si>
+  <si>
+    <t>Abhishekh Pandey</t>
+  </si>
+  <si>
+    <t>Shiddharth Khosla</t>
+  </si>
+  <si>
+    <t>Tanveer Khan</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Trisha Milind Patil </t>
+  </si>
+  <si>
+    <t>Shaunak Jadhav</t>
+  </si>
+  <si>
+    <t>Krish Gupta (BBA)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Arnav Akhil Rupji </t>
+  </si>
+  <si>
+    <t>Akul Tomar</t>
+  </si>
+  <si>
+    <t>BBA</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -291,16 +324,39 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1" tint="4.9989318521683403E-2"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF434343"/>
+      <name val="Roboto"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF8F9FA"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -308,36 +364,61 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="3">
+  <dxfs count="4">
     <dxf>
       <font>
-        <b val="0"/>
-        <i val="0"/>
         <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
         <outline val="0"/>
         <shadow val="0"/>
         <u val="none"/>
         <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color rgb="FF434343"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
+        <color theme="1"/>
       </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
       <font>
@@ -356,6 +437,12 @@
         <family val="2"/>
         <scheme val="none"/>
       </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
       <font>
@@ -374,6 +461,36 @@
         <family val="2"/>
         <scheme val="none"/>
       </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color rgb="FF434343"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -389,10 +506,10 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{0B9B57BC-9FDE-4251-9932-1C49163250DA}" name="Table1" displayName="Table1" ref="A1:D15" totalsRowShown="0">
-  <autoFilter ref="A1:D15" xr:uid="{0B9B57BC-9FDE-4251-9932-1C49163250DA}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{0B9B57BC-9FDE-4251-9932-1C49163250DA}" name="Table1" displayName="Table1" ref="A1:D19" totalsRowShown="0">
+  <autoFilter ref="A1:D19" xr:uid="{0B9B57BC-9FDE-4251-9932-1C49163250DA}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{48F2E2B7-FC60-4D1C-9399-2CDF2D9B2BFC}" name="Name"/>
+    <tableColumn id="1" xr3:uid="{48F2E2B7-FC60-4D1C-9399-2CDF2D9B2BFC}" name="Name" dataDxfId="0"/>
     <tableColumn id="2" xr3:uid="{C0083B03-192E-4C51-B3E5-6FA884241481}" name="Course"/>
     <tableColumn id="3" xr3:uid="{F8E03E2E-EACA-42AC-82E1-B3A228E18D95}" name="Payment"/>
     <tableColumn id="4" xr3:uid="{9602FABA-6558-4608-8DC3-346377C2B93E}" name="Mode"/>
@@ -405,7 +522,7 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{3201C194-DC57-483E-BDFD-A58C3B407816}" name="Table2" displayName="Table2" ref="A1:D16" totalsRowShown="0">
   <autoFilter ref="A1:D16" xr:uid="{3201C194-DC57-483E-BDFD-A58C3B407816}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{DC9BD4A4-6835-4E2A-B0CC-E60775C078B6}" name="Name" dataDxfId="2"/>
+    <tableColumn id="1" xr3:uid="{DC9BD4A4-6835-4E2A-B0CC-E60775C078B6}" name="Name" dataDxfId="1"/>
     <tableColumn id="2" xr3:uid="{91FBDB15-6C15-4286-B70C-C43CE063CD0B}" name="Course"/>
     <tableColumn id="3" xr3:uid="{4E136A08-EC4B-4321-BD71-10B75640FB93}" name="Payment"/>
     <tableColumn id="4" xr3:uid="{D6533733-D192-4E2C-9F7D-E28507DED2A4}" name="Mode"/>
@@ -415,10 +532,10 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{C504B386-A003-4888-9A26-A4972F488DF1}" name="Table3" displayName="Table3" ref="A1:D21" totalsRowShown="0">
-  <autoFilter ref="A1:D21" xr:uid="{C504B386-A003-4888-9A26-A4972F488DF1}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{C504B386-A003-4888-9A26-A4972F488DF1}" name="Table3" displayName="Table3" ref="A1:D25" totalsRowShown="0">
+  <autoFilter ref="A1:D25" xr:uid="{C504B386-A003-4888-9A26-A4972F488DF1}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{91BCF65C-84CB-43AB-BF7F-E53CF7D9A6D1}" name="Name" dataDxfId="1"/>
+    <tableColumn id="1" xr3:uid="{91BCF65C-84CB-43AB-BF7F-E53CF7D9A6D1}" name="Name" dataDxfId="2"/>
     <tableColumn id="2" xr3:uid="{A19C7122-EEC6-4982-960D-FD5E1E6C7C1D}" name="Course"/>
     <tableColumn id="3" xr3:uid="{D34B931B-8B4E-424E-BBAC-E2F9D4BB35DD}" name="Payment"/>
     <tableColumn id="4" xr3:uid="{2F5A9087-7170-4146-8ACC-7C643CE5D09C}" name="Mode"/>
@@ -428,10 +545,10 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{DC674854-7431-4CF4-86AA-594BC7B67C65}" name="Table4" displayName="Table4" ref="A1:D8" totalsRowShown="0">
-  <autoFilter ref="A1:D8" xr:uid="{DC674854-7431-4CF4-86AA-594BC7B67C65}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{DC674854-7431-4CF4-86AA-594BC7B67C65}" name="Table4" displayName="Table4" ref="A1:D10" totalsRowShown="0">
+  <autoFilter ref="A1:D10" xr:uid="{DC674854-7431-4CF4-86AA-594BC7B67C65}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{6DB82251-C9DF-4C11-B3B3-7EED9628ED28}" name="Name" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{6DB82251-C9DF-4C11-B3B3-7EED9628ED28}" name="Name" dataDxfId="3"/>
     <tableColumn id="2" xr3:uid="{B24496F3-F8EF-47D5-BA6C-8DEFF8ABE1BC}" name="Course"/>
     <tableColumn id="3" xr3:uid="{45E7BFCF-EB10-4593-9D97-F09EF09896CF}" name="Payment"/>
     <tableColumn id="4" xr3:uid="{4E04E494-3A39-44D9-82B0-AF49AEC0A27D}" name="Mode"/>
@@ -737,22 +854,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AAA3D827-78CE-4653-8D4B-C10AB394EBFC}">
-  <dimension ref="A1:D15"/>
+  <dimension ref="A1:D19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:D1048576"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.6640625" style="7" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.77734375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.21875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="8.21875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
+      <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
@@ -766,10 +883,10 @@
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
+      <c r="A2" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="3" t="s">
         <v>5</v>
       </c>
       <c r="C2">
@@ -780,10 +897,10 @@
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
+      <c r="A3" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="3" t="s">
         <v>8</v>
       </c>
       <c r="C3">
@@ -794,10 +911,10 @@
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
+      <c r="A4" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="3" t="s">
         <v>10</v>
       </c>
       <c r="C4">
@@ -808,10 +925,10 @@
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
+      <c r="A5" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="3" t="s">
         <v>12</v>
       </c>
       <c r="C5">
@@ -822,10 +939,10 @@
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
+      <c r="A6" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="3" t="s">
         <v>12</v>
       </c>
       <c r="C6">
@@ -836,10 +953,10 @@
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
+      <c r="A7" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="3" t="s">
         <v>15</v>
       </c>
       <c r="C7">
@@ -850,10 +967,10 @@
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
+      <c r="A8" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" s="3" t="s">
         <v>15</v>
       </c>
       <c r="C8">
@@ -864,24 +981,21 @@
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
+      <c r="A9" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C9">
-        <v>50</v>
-      </c>
-      <c r="D9" t="s">
-        <v>18</v>
+      <c r="C9" t="s">
+        <v>75</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
+      <c r="A10" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B10" s="3" t="s">
         <v>20</v>
       </c>
       <c r="C10">
@@ -892,10 +1006,10 @@
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
+      <c r="A11" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B11" s="3" t="s">
         <v>10</v>
       </c>
       <c r="C11">
@@ -906,10 +1020,10 @@
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
+      <c r="A12" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B12" s="3" t="s">
         <v>5</v>
       </c>
       <c r="C12">
@@ -920,10 +1034,10 @@
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
+      <c r="A13" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B13" s="3" t="s">
         <v>8</v>
       </c>
       <c r="C13">
@@ -934,27 +1048,86 @@
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
+      <c r="A14" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B14" s="3" t="s">
         <v>25</v>
+      </c>
+      <c r="C14">
+        <v>320</v>
       </c>
       <c r="D14" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A15" t="s">
+      <c r="A15" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B15" s="3" t="s">
         <v>20</v>
       </c>
       <c r="C15">
         <v>550</v>
       </c>
       <c r="D15" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A16" s="7" t="s">
+        <v>77</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="C16">
+        <v>550</v>
+      </c>
+      <c r="D16" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A17" s="9" t="s">
+        <v>82</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C17">
+        <v>110</v>
+      </c>
+      <c r="D17" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A18" s="9" t="s">
+        <v>84</v>
+      </c>
+      <c r="B18" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C18">
+        <v>110</v>
+      </c>
+      <c r="D18" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A19" s="9" t="s">
+        <v>85</v>
+      </c>
+      <c r="B19" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="C19">
+        <v>110</v>
+      </c>
+      <c r="D19" t="s">
         <v>6</v>
       </c>
     </row>
@@ -968,22 +1141,24 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CAA723B1-C27C-4B8B-9218-FB3F8CACF8BD}">
-  <dimension ref="A1:D16"/>
+  <dimension ref="A1:J16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:D1048576"/>
+      <selection sqref="A1:A1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="16.88671875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18" style="7" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10.77734375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="8.21875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="8.88671875" customWidth="1"/>
+    <col min="10" max="10" width="10" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
@@ -996,9 +1171,9 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A2" s="1" t="s">
-        <v>27</v>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A2" s="8" t="s">
+        <v>76</v>
       </c>
       <c r="B2" t="s">
         <v>25</v>
@@ -1010,9 +1185,9 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A3" s="1" t="s">
-        <v>28</v>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A3" s="8" t="s">
+        <v>27</v>
       </c>
       <c r="B3" t="s">
         <v>12</v>
@@ -1024,9 +1199,9 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A4" s="1" t="s">
-        <v>29</v>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A4" s="8" t="s">
+        <v>28</v>
       </c>
       <c r="B4" t="s">
         <v>20</v>
@@ -1038,12 +1213,12 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A5" s="1" t="s">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A5" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="B5" t="s">
         <v>30</v>
-      </c>
-      <c r="B5" t="s">
-        <v>31</v>
       </c>
       <c r="C5">
         <v>300</v>
@@ -1052,12 +1227,12 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A6" s="1" t="s">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A6" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="B6" t="s">
         <v>32</v>
-      </c>
-      <c r="B6" t="s">
-        <v>33</v>
       </c>
       <c r="C6">
         <v>350</v>
@@ -1066,23 +1241,23 @@
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A7" s="1" t="s">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A7" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="B7" t="s">
         <v>34</v>
       </c>
-      <c r="B7" t="s">
+      <c r="C7">
+        <v>50</v>
+      </c>
+      <c r="D7" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A8" s="8" t="s">
         <v>35</v>
-      </c>
-      <c r="C7">
-        <v>50</v>
-      </c>
-      <c r="D7" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A8" s="1" t="s">
-        <v>36</v>
       </c>
       <c r="B8" t="s">
         <v>25</v>
@@ -1094,9 +1269,9 @@
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A9" s="1" t="s">
-        <v>37</v>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A9" s="8" t="s">
+        <v>36</v>
       </c>
       <c r="B9" t="s">
         <v>12</v>
@@ -1108,12 +1283,12 @@
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A10" s="1" t="s">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A10" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="B10" t="s">
         <v>38</v>
-      </c>
-      <c r="B10" t="s">
-        <v>39</v>
       </c>
       <c r="C10">
         <v>50</v>
@@ -1122,23 +1297,24 @@
         <v>18</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A11" s="1" t="s">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A11" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="B11" t="s">
+        <v>34</v>
+      </c>
+      <c r="C11">
+        <v>50</v>
+      </c>
+      <c r="D11" t="s">
+        <v>6</v>
+      </c>
+      <c r="J11" s="2"/>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A12" s="8" t="s">
         <v>40</v>
-      </c>
-      <c r="B11" t="s">
-        <v>35</v>
-      </c>
-      <c r="C11">
-        <v>50</v>
-      </c>
-      <c r="D11" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A12" s="1" t="s">
-        <v>41</v>
       </c>
       <c r="B12" t="s">
         <v>15</v>
@@ -1150,9 +1326,9 @@
         <v>6</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A13" s="1" t="s">
-        <v>42</v>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A13" s="10" t="s">
+        <v>41</v>
       </c>
       <c r="B13" t="s">
         <v>10</v>
@@ -1164,9 +1340,9 @@
         <v>6</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A14" s="1" t="s">
-        <v>43</v>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A14" s="8" t="s">
+        <v>42</v>
       </c>
       <c r="B14" t="s">
         <v>5</v>
@@ -1178,20 +1354,23 @@
         <v>6</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A15" s="1" t="s">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A15" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="B15" t="s">
         <v>44</v>
       </c>
-      <c r="B15" t="s">
-        <v>45</v>
+      <c r="C15">
+        <v>350</v>
       </c>
       <c r="D15" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A16" s="1" t="s">
-        <v>46</v>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A16" s="8" t="s">
+        <v>45</v>
       </c>
       <c r="B16" t="s">
         <v>12</v>
@@ -1213,22 +1392,22 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F13D3714-DC80-4C4E-9F61-5ADFBB4FB644}">
-  <dimension ref="A1:D21"/>
+  <dimension ref="A1:G25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:D1048576"/>
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="20.88671875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.88671875" style="7" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10.77734375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="8.21875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
@@ -1241,23 +1420,24 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A2" s="1" t="s">
-        <v>47</v>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A2" s="8" t="s">
+        <v>46</v>
       </c>
       <c r="B2" t="s">
         <v>8</v>
       </c>
       <c r="C2">
-        <v>200</v>
+        <v>100</v>
       </c>
       <c r="D2" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A3" s="1" t="s">
-        <v>48</v>
+      <c r="G2" s="1"/>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A3" s="8" t="s">
+        <v>47</v>
       </c>
       <c r="B3" t="s">
         <v>12</v>
@@ -1268,10 +1448,11 @@
       <c r="D3" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A4" s="1" t="s">
-        <v>49</v>
+      <c r="G3" s="1"/>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A4" s="8" t="s">
+        <v>48</v>
       </c>
       <c r="B4" t="s">
         <v>12</v>
@@ -1282,35 +1463,41 @@
       <c r="D4" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A5" s="1" t="s">
-        <v>50</v>
+      <c r="G4" s="1"/>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A5" s="8" t="s">
+        <v>49</v>
       </c>
       <c r="B5" t="s">
         <v>15</v>
       </c>
+      <c r="C5">
+        <v>200</v>
+      </c>
       <c r="D5" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A6" s="1" t="s">
+      <c r="G5" s="1"/>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A6" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="B6" t="s">
         <v>51</v>
       </c>
-      <c r="B6" t="s">
+      <c r="C6">
+        <v>50</v>
+      </c>
+      <c r="D6" t="s">
+        <v>6</v>
+      </c>
+      <c r="G6" s="1"/>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A7" s="8" t="s">
         <v>52</v>
-      </c>
-      <c r="C6">
-        <v>50</v>
-      </c>
-      <c r="D6" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A7" s="1" t="s">
-        <v>53</v>
       </c>
       <c r="B7" t="s">
         <v>8</v>
@@ -1321,13 +1508,14 @@
       <c r="D7" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A8" s="1" t="s">
-        <v>54</v>
+      <c r="G7" s="6"/>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A8" s="8" t="s">
+        <v>53</v>
       </c>
       <c r="B8" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C8">
         <v>150</v>
@@ -1335,63 +1523,71 @@
       <c r="D8" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A9" s="1" t="s">
-        <v>55</v>
+      <c r="G8" s="1"/>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A9" s="8" t="s">
+        <v>54</v>
       </c>
       <c r="B9" t="s">
         <v>12</v>
       </c>
+      <c r="C9">
+        <v>50</v>
+      </c>
       <c r="D9" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A10" s="1" t="s">
+      <c r="G9" s="1"/>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A10" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="B10" t="s">
+        <v>51</v>
+      </c>
+      <c r="C10">
+        <v>50</v>
+      </c>
+      <c r="D10" t="s">
+        <v>6</v>
+      </c>
+      <c r="G10" s="1"/>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A11" s="8" t="s">
         <v>56</v>
       </c>
-      <c r="B10" t="s">
-        <v>52</v>
-      </c>
-      <c r="C10">
-        <v>50</v>
-      </c>
-      <c r="D10" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A11" s="1" t="s">
+      <c r="B11" t="s">
+        <v>51</v>
+      </c>
+      <c r="C11">
+        <v>50</v>
+      </c>
+      <c r="D11" t="s">
+        <v>6</v>
+      </c>
+      <c r="G11" s="1"/>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A12" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="B11" t="s">
-        <v>52</v>
-      </c>
-      <c r="C11">
-        <v>50</v>
-      </c>
-      <c r="D11" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A12" s="1" t="s">
+      <c r="B12" t="s">
+        <v>64</v>
+      </c>
+      <c r="C12">
+        <v>50</v>
+      </c>
+      <c r="D12" t="s">
+        <v>6</v>
+      </c>
+      <c r="G12" s="1"/>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A13" s="8" t="s">
         <v>58</v>
-      </c>
-      <c r="B12" t="s">
-        <v>65</v>
-      </c>
-      <c r="C12">
-        <v>50</v>
-      </c>
-      <c r="D12" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A13" s="1" t="s">
-        <v>59</v>
       </c>
       <c r="B13" t="s">
         <v>10</v>
@@ -1402,21 +1598,26 @@
       <c r="D13" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A14" s="1" t="s">
+      <c r="G13" s="1"/>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A14" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="B14" t="s">
         <v>30</v>
       </c>
-      <c r="B14" t="s">
-        <v>31</v>
+      <c r="C14">
+        <v>200</v>
       </c>
       <c r="D14" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A15" s="1" t="s">
-        <v>66</v>
+      <c r="G14" s="1"/>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A15" s="8" t="s">
+        <v>65</v>
       </c>
       <c r="B15" t="s">
         <v>10</v>
@@ -1427,10 +1628,11 @@
       <c r="D15" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A16" s="1" t="s">
-        <v>60</v>
+      <c r="G15" s="1"/>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A16" s="8" t="s">
+        <v>59</v>
       </c>
       <c r="B16" t="s">
         <v>5</v>
@@ -1441,32 +1643,41 @@
       <c r="D16" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A17" s="1" t="s">
-        <v>61</v>
+      <c r="G16" s="1"/>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A17" s="8" t="s">
+        <v>60</v>
       </c>
       <c r="B17" t="s">
-        <v>45</v>
+        <v>44</v>
+      </c>
+      <c r="C17">
+        <v>200</v>
       </c>
       <c r="D17" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A18" s="1" t="s">
-        <v>62</v>
+      <c r="G17" s="1"/>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A18" s="8" t="s">
+        <v>61</v>
       </c>
       <c r="B18" t="s">
         <v>8</v>
       </c>
+      <c r="C18">
+        <v>200</v>
+      </c>
       <c r="D18" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A19" s="1" t="s">
-        <v>63</v>
+      <c r="G18" s="1"/>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A19" s="8" t="s">
+        <v>62</v>
       </c>
       <c r="B19" t="s">
         <v>5</v>
@@ -1477,10 +1688,11 @@
       <c r="D19" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A20" s="2" t="s">
-        <v>67</v>
+      <c r="G19" s="1"/>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A20" s="9" t="s">
+        <v>66</v>
       </c>
       <c r="B20" t="s">
         <v>8</v>
@@ -1491,10 +1703,11 @@
       <c r="D20" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A21" s="1" t="s">
-        <v>64</v>
+      <c r="G20" s="1"/>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A21" s="8" t="s">
+        <v>63</v>
       </c>
       <c r="B21" t="s">
         <v>8</v>
@@ -1503,6 +1716,64 @@
         <v>200</v>
       </c>
       <c r="D21" t="s">
+        <v>6</v>
+      </c>
+      <c r="G21" s="1"/>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A22" s="8" t="s">
+        <v>78</v>
+      </c>
+      <c r="B22" t="s">
+        <v>20</v>
+      </c>
+      <c r="C22">
+        <v>150</v>
+      </c>
+      <c r="D22" t="s">
+        <v>6</v>
+      </c>
+      <c r="G22" s="1"/>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A23" s="8" t="s">
+        <v>79</v>
+      </c>
+      <c r="B23" t="s">
+        <v>38</v>
+      </c>
+      <c r="C23">
+        <v>50</v>
+      </c>
+      <c r="D23" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A24" s="8" t="s">
+        <v>80</v>
+      </c>
+      <c r="B24" t="s">
+        <v>38</v>
+      </c>
+      <c r="C24">
+        <v>50</v>
+      </c>
+      <c r="D24" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A25" s="8" t="s">
+        <v>81</v>
+      </c>
+      <c r="B25" t="s">
+        <v>38</v>
+      </c>
+      <c r="C25">
+        <v>50</v>
+      </c>
+      <c r="D25" t="s">
         <v>6</v>
       </c>
     </row>
@@ -1516,22 +1787,22 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4E48DB26-85C5-4A28-A407-2B4B13E9FAA5}">
-  <dimension ref="A1:D8"/>
+  <dimension ref="A1:J13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="33.77734375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="33.77734375" style="7" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="15.6640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="8.21875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
@@ -1544,9 +1815,9 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>68</v>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A2" s="7" t="s">
+        <v>67</v>
       </c>
       <c r="B2" t="s">
         <v>12</v>
@@ -1558,20 +1829,20 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A3" s="1" t="s">
-        <v>69</v>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A3" s="8" t="s">
+        <v>68</v>
       </c>
       <c r="B3" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="C3" s="2" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A4" s="8" t="s">
         <v>70</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A4" s="1" t="s">
-        <v>71</v>
       </c>
       <c r="B4" t="s">
         <v>8</v>
@@ -1583,9 +1854,9 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A5" s="1" t="s">
-        <v>72</v>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A5" s="8" t="s">
+        <v>71</v>
       </c>
       <c r="B5" t="s">
         <v>12</v>
@@ -1597,12 +1868,12 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A6" s="1" t="s">
-        <v>73</v>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A6" s="8" t="s">
+        <v>72</v>
       </c>
       <c r="B6" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C6">
         <v>100</v>
@@ -1611,23 +1882,27 @@
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A7" s="1" t="s">
-        <v>74</v>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A7" s="8" t="s">
+        <v>73</v>
       </c>
       <c r="B7" t="s">
         <v>12</v>
       </c>
+      <c r="C7">
+        <v>50</v>
+      </c>
       <c r="D7" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A8" s="1" t="s">
-        <v>75</v>
+      <c r="J7" s="1"/>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A8" s="8" t="s">
+        <v>74</v>
       </c>
       <c r="B8" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C8">
         <v>200</v>
@@ -1635,6 +1910,43 @@
       <c r="D8" t="s">
         <v>6</v>
       </c>
+      <c r="J8" s="1"/>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A9" s="8" t="s">
+        <v>79</v>
+      </c>
+      <c r="B9" t="s">
+        <v>38</v>
+      </c>
+      <c r="C9">
+        <v>50</v>
+      </c>
+      <c r="D9" t="s">
+        <v>6</v>
+      </c>
+      <c r="J9" s="1"/>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A10" s="8" t="s">
+        <v>83</v>
+      </c>
+      <c r="B10" t="s">
+        <v>86</v>
+      </c>
+      <c r="C10">
+        <v>250</v>
+      </c>
+      <c r="D10" t="s">
+        <v>6</v>
+      </c>
+      <c r="J10" s="1"/>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="J11" s="1"/>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="J13" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>